<commit_message>
final scraper with yelp
</commit_message>
<xml_diff>
--- a/df_Review_BK.xlsx
+++ b/df_Review_BK.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D256"/>
+  <dimension ref="A1:D477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5140,6 +5140,4171 @@
         </is>
       </c>
     </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B257" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B258" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B259" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B260" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B261" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B262" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B263" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B264" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B265" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B266" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B267" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B268" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B269" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B270" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B271" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B272" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B273" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B274" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B275" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B276" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B277" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B278" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B279" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B280" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B281" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B282" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B283" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B284" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B285" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B286" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B287" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B288" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B289" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B290" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B291" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B292" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B293" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B294" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B295" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B296" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B297" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B298" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B299" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B300" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B301" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B302" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B303" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B304" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B305" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B306" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B307" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B308" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B309" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B310" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B311" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B312" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B313" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B314" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B315" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B316" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B317" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B318" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B319" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B320" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B321" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B322" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B323" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B324" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B325" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B326" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B327" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="B328" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B329" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B330" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="B331" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="B332" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="B333" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="B334" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>332</v>
+      </c>
+      <c r="B335" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="B336" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B337" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>335</v>
+      </c>
+      <c r="B338" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="B339" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>337</v>
+      </c>
+      <c r="B340" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="B341" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B342" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B343" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B344" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B345" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="B346" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B347" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="B348" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="B349" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>347</v>
+      </c>
+      <c r="B350" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="B351" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="B352" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B353" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B354" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B355" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="B356" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B357" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="B358" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="B359" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B360" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="B361" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="B362" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B363" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="B364" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>362</v>
+      </c>
+      <c r="B365" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>363</v>
+      </c>
+      <c r="B366" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>364</v>
+      </c>
+      <c r="B367" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="B368" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="B369" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="B370" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="B371" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="B372" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="B373" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="B374" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="B375" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="B376" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="B377" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="B378" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="B379" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="B380" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="B381" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="n">
+        <v>379</v>
+      </c>
+      <c r="B382" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="B383" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="n">
+        <v>381</v>
+      </c>
+      <c r="B384" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="n">
+        <v>382</v>
+      </c>
+      <c r="B385" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="n">
+        <v>383</v>
+      </c>
+      <c r="B386" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1" t="n">
+        <v>384</v>
+      </c>
+      <c r="B387" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="B388" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1" t="n">
+        <v>386</v>
+      </c>
+      <c r="B389" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1" t="n">
+        <v>387</v>
+      </c>
+      <c r="B390" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="n">
+        <v>388</v>
+      </c>
+      <c r="B391" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1" t="n">
+        <v>389</v>
+      </c>
+      <c r="B392" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1" t="n">
+        <v>390</v>
+      </c>
+      <c r="B393" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="n">
+        <v>391</v>
+      </c>
+      <c r="B394" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="n">
+        <v>392</v>
+      </c>
+      <c r="B395" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1" t="n">
+        <v>393</v>
+      </c>
+      <c r="B396" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="n">
+        <v>394</v>
+      </c>
+      <c r="B397" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="n">
+        <v>395</v>
+      </c>
+      <c r="B398" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="n">
+        <v>396</v>
+      </c>
+      <c r="B399" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>397</v>
+      </c>
+      <c r="B400" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="B401" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>399</v>
+      </c>
+      <c r="B402" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="B403" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="n">
+        <v>401</v>
+      </c>
+      <c r="B404" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="n">
+        <v>402</v>
+      </c>
+      <c r="B405" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1" t="n">
+        <v>403</v>
+      </c>
+      <c r="B406" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1" t="n">
+        <v>404</v>
+      </c>
+      <c r="B407" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1" t="n">
+        <v>405</v>
+      </c>
+      <c r="B408" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1" t="n">
+        <v>406</v>
+      </c>
+      <c r="B409" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1" t="n">
+        <v>407</v>
+      </c>
+      <c r="B410" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B411" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="1" t="n">
+        <v>409</v>
+      </c>
+      <c r="B412" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1" t="n">
+        <v>410</v>
+      </c>
+      <c r="B413" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="1" t="n">
+        <v>411</v>
+      </c>
+      <c r="B414" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1" t="n">
+        <v>412</v>
+      </c>
+      <c r="B415" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1" t="n">
+        <v>413</v>
+      </c>
+      <c r="B416" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1" t="n">
+        <v>414</v>
+      </c>
+      <c r="B417" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1" t="n">
+        <v>415</v>
+      </c>
+      <c r="B418" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1" t="n">
+        <v>416</v>
+      </c>
+      <c r="B419" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1" t="n">
+        <v>417</v>
+      </c>
+      <c r="B420" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1" t="n">
+        <v>418</v>
+      </c>
+      <c r="B421" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1" t="n">
+        <v>419</v>
+      </c>
+      <c r="B422" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="B423" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="1" t="n">
+        <v>421</v>
+      </c>
+      <c r="B424" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="1" t="n">
+        <v>422</v>
+      </c>
+      <c r="B425" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="1" t="n">
+        <v>423</v>
+      </c>
+      <c r="B426" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="1" t="n">
+        <v>424</v>
+      </c>
+      <c r="B427" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="1" t="n">
+        <v>425</v>
+      </c>
+      <c r="B428" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="1" t="n">
+        <v>426</v>
+      </c>
+      <c r="B429" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="B430" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="1" t="n">
+        <v>428</v>
+      </c>
+      <c r="B431" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="1" t="n">
+        <v>429</v>
+      </c>
+      <c r="B432" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="1" t="n">
+        <v>430</v>
+      </c>
+      <c r="B433" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="1" t="n">
+        <v>431</v>
+      </c>
+      <c r="B434" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="1" t="n">
+        <v>432</v>
+      </c>
+      <c r="B435" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="1" t="n">
+        <v>433</v>
+      </c>
+      <c r="B436" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="1" t="n">
+        <v>434</v>
+      </c>
+      <c r="B437" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="1" t="n">
+        <v>435</v>
+      </c>
+      <c r="B438" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1" t="n">
+        <v>436</v>
+      </c>
+      <c r="B439" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="1" t="n">
+        <v>437</v>
+      </c>
+      <c r="B440" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="1" t="n">
+        <v>438</v>
+      </c>
+      <c r="B441" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="1" t="n">
+        <v>439</v>
+      </c>
+      <c r="B442" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="1" t="n">
+        <v>440</v>
+      </c>
+      <c r="B443" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="1" t="n">
+        <v>441</v>
+      </c>
+      <c r="B444" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="1" t="n">
+        <v>442</v>
+      </c>
+      <c r="B445" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="B446" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="1" t="n">
+        <v>444</v>
+      </c>
+      <c r="B447" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="1" t="n">
+        <v>445</v>
+      </c>
+      <c r="B448" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="1" t="n">
+        <v>446</v>
+      </c>
+      <c r="B449" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="1" t="n">
+        <v>447</v>
+      </c>
+      <c r="B450" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="1" t="n">
+        <v>448</v>
+      </c>
+      <c r="B451" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1" t="n">
+        <v>449</v>
+      </c>
+      <c r="B452" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="1" t="n">
+        <v>450</v>
+      </c>
+      <c r="B453" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="1" t="n">
+        <v>451</v>
+      </c>
+      <c r="B454" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="1" t="n">
+        <v>452</v>
+      </c>
+      <c r="B455" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1" t="n">
+        <v>453</v>
+      </c>
+      <c r="B456" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1" t="n">
+        <v>454</v>
+      </c>
+      <c r="B457" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1" t="n">
+        <v>455</v>
+      </c>
+      <c r="B458" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="B459" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="1" t="n">
+        <v>457</v>
+      </c>
+      <c r="B460" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="1" t="n">
+        <v>458</v>
+      </c>
+      <c r="B461" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="1" t="n">
+        <v>459</v>
+      </c>
+      <c r="B462" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="1" t="n">
+        <v>460</v>
+      </c>
+      <c r="B463" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="1" t="n">
+        <v>461</v>
+      </c>
+      <c r="B464" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="1" t="n">
+        <v>462</v>
+      </c>
+      <c r="B465" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>The double whopper is not bad the food definitely is better then the states, I would go back the staff is friendly too .</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="1" t="n">
+        <v>463</v>
+      </c>
+      <c r="B466" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>Almost everything ok. The order came right and the staff was friendly. However, It took about 20 minutes for the order to arrive, which is quite slow for a fast food joint.</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="1" t="n">
+        <v>464</v>
+      </c>
+      <c r="B467" s="2" t="n">
+        <v>43298</v>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>Prime location which gets a lot of traffic. I liked the cheddar whopper and found it better than we get back home in the States.</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="1" t="n">
+        <v>465</v>
+      </c>
+      <c r="B468" s="2" t="n">
+        <v>42465</v>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>food is your usual run of the mill Burger King standard. This place is great for a quick bite that is cheap and cheerful in the heart of the West End. Whether you have a few mins to spare or just want to dine and dash. Because of where it is, it gets very very busy and sometimes the staff are overwhelmed hence service isnt always up to scratch but they are doing there best.
+ If you are there for a film premiere its great as its just opposite the cinema.</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="1" t="n">
+        <v>466</v>
+      </c>
+      <c r="B469" s="2" t="n">
+        <v>43814</v>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>Disgusting place to eat. Extremely poor service and staff extremely rude. Security treats customers as cattle. Stay away</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="1" t="n">
+        <v>467</v>
+      </c>
+      <c r="B470" s="2" t="n">
+        <v>41996</v>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>What the hell is happening here please? 
+As a Belgian tourist, I&amp;apos;m &amp;quot;obliged&amp;quot; to travel abroad to be able to enjoy a Burger King... You, people of London, have like one BK in each main street of the city and we, poor Belgian people, have no burger place in town! Life is so unfair sometimes...  
+However, if we get one in Brussels one day, if it is one such as the BK on Leicester Square, you now what? You can keep it! This place is just horrible: sticky floor (chairs and tables), dirty tables full of garbage, pathetic staff who stops you in the middle of your order to serve family members who just arrived and this for a bargain price compared to your addition, many oversights (forgetting to give the ketchup is not a big deal but forgetting a burger... seriously?). 
+In short, I will never come back here, it is crystal clear !</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="1" t="n">
+        <v>468</v>
+      </c>
+      <c r="B471" s="2" t="n">
+        <v>42232</v>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>Terrible service. Employees yelling at each other and complaining in front of us. We came for breakfast and there was no line -- there was by the time we finally got our order placed. Never return.</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="B472" s="2" t="n">
+        <v>40232</v>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>Like any French when we go to UK we eat in Burger King because we aren&amp;apos;t lucky and unfortunately we haven&amp;apos;t this brand in our lovely country :)
+This Burger King is pretty big. It&amp;apos;s always crowed. 
+In my opinion, I always take the Wooper and here you can find the triple Wooper.
+It&amp;apos;s not expensive and you can eat for only 6£.
+ However, I can&amp;apos;t put more 3 stars it&amp;apos;s a junk food :)</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1" t="n">
+        <v>470</v>
+      </c>
+      <c r="B473" s="2" t="n">
+        <v>40661</v>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>Bacon double cheese burger. All I need to say.
+ I really like this burger king. Excellent location right in the heart of Leicester square - always open late.
+ I know the chips are no comparison to Mac Donalds, but the burgers win hands down.</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B474" s="2" t="n">
+        <v>41978</v>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>I won&amp;apos;t go back! The food is not bad, so this is an Operations and Marketing review. There is zero customer service, rude staff, no proper ordering system. Trying to order is just a free for all with staff behind the counter just screaming. Not enough seating, people are just standing with their trays of food waiting for a table. When you finally get a table, it&amp;apos;s dirty! 
+So BK has an ad on TV boasting a really big BK meal for £3.79. Surprise surprise, it&amp;apos;s not even advertised on the menu. I had a meat lovers whopper and came to £7.39. I asked the server taking my order if there was cheese on the meat lovers whopper and I was told yes. Well, there actually was NO cheese on it. Server could hardly speak English! Geez Burger King, get your marketing act together for crying out loud and sort your outlets out. There are so many up and coming burger outlets which are far better and will put you out of business if things don&amp;apos;t improve. Netflix did it to Blockbuster and Netflix was started by an irate customer like myself!</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1" t="n">
+        <v>472</v>
+      </c>
+      <c r="B475" s="2" t="n">
+        <v>39960</v>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>Burger King Leicester Square is perfect for the square if you are on a budget. This is tourism central as far as London goes and for under five pounds you can get a meal that will fill you up. In my opinion, much better than McDonalds which is also near by, and a lot better than the dodgy pizza just round the corner.</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="n">
+        <v>473</v>
+      </c>
+      <c r="B476" s="2" t="n">
+        <v>41311</v>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>late night eating place when you tipsy and hungry.. they should stop employing rude security guards who can not speak English (only F words)!!!</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="n">
+        <v>474</v>
+      </c>
+      <c r="B477" s="2" t="n">
+        <v>40352</v>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>The Angus Burger Is The Greatest thing ever invented. Don&amp;apos;t ever take this thing out of my life!!!</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>Yelp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>